<commit_message>
Analisis binaria y graficas comparacion
</commit_message>
<xml_diff>
--- a/Practica2/Pruebas/Pruebas.xlsx
+++ b/Practica2/Pruebas/Pruebas.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abigail\Desktop\ESCUELA\GitHub\Analisis-Algoritmos\Practica2\Pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YaKerTaker\Google Drive\5° SEMESTRE\Analisis de Algoritmos\Practicas\Practica2\Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94CD2D0-38D4-430C-AE6F-89FBB59F1360}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A53686-677C-4512-93BD-31A1E1C024F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3495" activeTab="2" xr2:uid="{0F44E7D9-DF95-46A6-BB1E-3FAAE9BCBC95}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3495" activeTab="3" xr2:uid="{0F44E7D9-DF95-46A6-BB1E-3FAAE9BCBC95}"/>
   </bookViews>
   <sheets>
     <sheet name="Binaria" sheetId="1" r:id="rId1"/>
     <sheet name="Lineal" sheetId="2" r:id="rId2"/>
     <sheet name="ABB" sheetId="3" r:id="rId3"/>
+    <sheet name="Comparativa" sheetId="4" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="179021"/>
   <extLst>
@@ -3447,6 +3448,885 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Lineal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ABB!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Lineal!$H$2:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>8.7022783645807003E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.77757635558373E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.569986307004E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1076202756375999E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.00839140941388E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9055604934692299E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.7535428418777802E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.3131325189024199E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2246966361999501E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6656507980078398E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.82319874875247E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.6878467071801398E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.28765812143683E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.3069212958216598E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.9125625565647992E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.11029148101806E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.25129465013742E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4274966903030799E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5519404783844899E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.7345856875181101E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B99B-4C6B-9F8E-4530D90973B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Binaria</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ABB!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Binaria!$H$2:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.6757201011568996E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5101854690728995E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5565109252930005E-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.9604644775390996E-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.4638594444186003E-7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.9870221725287001E-7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.0599058921725002E-7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.4638594444186003E-7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.3909757247748002E-7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.4175339881985999E-7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.1525573730469004E-7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1563300859052099E-6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.09672544112982E-6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.13248825073242E-6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.10864641555963E-6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.2636185147130199E-6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.2755393754559899E-6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.2874603498858099E-6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2636185147130199E-6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.3828278042637999E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B99B-4C6B-9F8E-4530D90973B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>ABB</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ABB!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ABB!$H$2:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.4373017494289998E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0796736534029997E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.9604644775390996E-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0333481971828997E-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5367431640625E-7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.3909757247748002E-7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2040138699376299E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.9219858081196401E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1205672763026099E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.19209289550781E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5020370938145799E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5020370938145799E-6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5854835737627601E-6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.69277188888373E-6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.63316724410834E-6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.1219252630544399E-6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.85966496246692E-6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8358230136073E-6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.4213067010568899E-6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.8358230136073E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B99B-4C6B-9F8E-4530D90973B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="499859416"/>
+        <c:axId val="499863024"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="499859416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="499863024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="499863024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0000000000000004E-5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>TIEMPO</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> (SEG)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="499859416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1.0000000000000004E-6"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3647,6 +4527,43 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -5660,6 +6577,509 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6347,6 +7767,47 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123824</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0646456B-9828-4760-B459-9EF1110BFD89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -7001,7 +8462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E75AF09-E0BD-4AA2-AB32-F0D8724F4C46}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
@@ -8183,7 +9644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D766D3-7DAB-4C17-B436-DF4198543227}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -9365,7 +10826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C816D298-396B-4A20-B39E-B7A0B315C873}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
@@ -9932,4 +11393,19 @@
   </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2381FC31-2AB0-41D8-B87B-E77E61F8954D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>